<commit_message>
First adjustments: Blade, Inertia, DLC1.4, 1.3, 5.1
All three DLC's have no changed torque controler parameters
</commit_message>
<xml_diff>
--- a/IEA-3.4-130-RWT/IEA_HH140_D178/DLC_1_4/Wind_preperation.xlsx
+++ b/IEA-3.4-130-RWT/IEA_HH140_D178/DLC_1_4/Wind_preperation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\GitHub\Optimus2024\IEA-3.4-130-RWT\IEA_HH140_D178\DLC_1_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3700895A-8A47-4328-A249-A719AA4A5A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439A7838-A670-4D82-A8C1-A11A1AB29C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BB01B48E-3559-49FD-94B4-E017B99DE7F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{BB01B48E-3559-49FD-94B4-E017B99DE7F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -148,7 +148,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -6895,7 +6895,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6973,8 +6973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B080A3CF-4F71-41D8-81CB-4A772A265761}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="58" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:I20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7656,7 +7656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7204C4B4-D35C-4EA3-9CAC-EB4CB6F0EF4D}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="54" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>

</xml_diff>